<commit_message>
ferdig kontoret, resten skriving
</commit_message>
<xml_diff>
--- a/Kode/Server2/Logs/lora_node3/2020-06-08.xlsx
+++ b/Kode/Server2/Logs/lora_node3/2020-06-08.xlsx
@@ -346,7 +346,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F287"/>
+  <dimension ref="A1:F408"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6106,6 +6106,2426 @@
         <v>0.6384</v>
       </c>
     </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>230</v>
+      </c>
+      <c r="B288" s="1" t="n">
+        <v>0.7979885175462963</v>
+      </c>
+      <c r="C288" t="n">
+        <v>84</v>
+      </c>
+      <c r="D288" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="E288" t="n">
+        <v>8.94</v>
+      </c>
+      <c r="F288" t="n">
+        <v>0.7151999999999999</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>231</v>
+      </c>
+      <c r="B289" s="1" t="n">
+        <v>0.7986807903356482</v>
+      </c>
+      <c r="C289" t="n">
+        <v>84</v>
+      </c>
+      <c r="D289" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="E289" t="n">
+        <v>9.014999999999999</v>
+      </c>
+      <c r="F289" t="n">
+        <v>0.7212</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>232</v>
+      </c>
+      <c r="B290" s="1" t="n">
+        <v>0.7993754661226853</v>
+      </c>
+      <c r="C290" t="n">
+        <v>84</v>
+      </c>
+      <c r="D290" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="E290" t="n">
+        <v>9.014999999999999</v>
+      </c>
+      <c r="F290" t="n">
+        <v>0.7212</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>234</v>
+      </c>
+      <c r="B291" s="1" t="n">
+        <v>0.8007614704861111</v>
+      </c>
+      <c r="C291" t="n">
+        <v>84</v>
+      </c>
+      <c r="D291" t="n">
+        <v>0.08400000000000001</v>
+      </c>
+      <c r="E291" t="n">
+        <v>9.359999999999999</v>
+      </c>
+      <c r="F291" t="n">
+        <v>0.78624</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>236</v>
+      </c>
+      <c r="B292" s="1" t="n">
+        <v>0.8021540336689814</v>
+      </c>
+      <c r="C292" t="n">
+        <v>84</v>
+      </c>
+      <c r="D292" t="n">
+        <v>0.08400000000000001</v>
+      </c>
+      <c r="E292" t="n">
+        <v>9.539999999999999</v>
+      </c>
+      <c r="F292" t="n">
+        <v>0.80136</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>242</v>
+      </c>
+      <c r="B293" s="1" t="n">
+        <v>0.806315097662037</v>
+      </c>
+      <c r="C293" t="n">
+        <v>84</v>
+      </c>
+      <c r="D293" t="n">
+        <v>0.08400000000000001</v>
+      </c>
+      <c r="E293" t="n">
+        <v>9.48</v>
+      </c>
+      <c r="F293" t="n">
+        <v>0.7963200000000001</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>248</v>
+      </c>
+      <c r="B294" s="1" t="n">
+        <v>0.8104790237268519</v>
+      </c>
+      <c r="C294" t="n">
+        <v>84</v>
+      </c>
+      <c r="D294" t="n">
+        <v>0.076</v>
+      </c>
+      <c r="E294" t="n">
+        <v>8.625</v>
+      </c>
+      <c r="F294" t="n">
+        <v>0.6555</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>249</v>
+      </c>
+      <c r="B295" s="1" t="n">
+        <v>0.8111736644097223</v>
+      </c>
+      <c r="C295" t="n">
+        <v>84</v>
+      </c>
+      <c r="D295" t="n">
+        <v>0.076</v>
+      </c>
+      <c r="E295" t="n">
+        <v>8.549999999999999</v>
+      </c>
+      <c r="F295" t="n">
+        <v>0.6497999999999999</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>250</v>
+      </c>
+      <c r="B296" s="1" t="n">
+        <v>0.8118673618055556</v>
+      </c>
+      <c r="C296" t="n">
+        <v>84</v>
+      </c>
+      <c r="D296" t="n">
+        <v>0.07200000000000001</v>
+      </c>
+      <c r="E296" t="n">
+        <v>8.369999999999999</v>
+      </c>
+      <c r="F296" t="n">
+        <v>0.6026400000000001</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>251</v>
+      </c>
+      <c r="B297" s="1" t="n">
+        <v>0.8125632428472221</v>
+      </c>
+      <c r="C297" t="n">
+        <v>84</v>
+      </c>
+      <c r="D297" t="n">
+        <v>0.07200000000000001</v>
+      </c>
+      <c r="E297" t="n">
+        <v>8.055</v>
+      </c>
+      <c r="F297" t="n">
+        <v>0.57996</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>252</v>
+      </c>
+      <c r="B298" s="1" t="n">
+        <v>0.8132560239699074</v>
+      </c>
+      <c r="C298" t="n">
+        <v>84</v>
+      </c>
+      <c r="D298" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="E298" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="F298" t="n">
+        <v>0.5304</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>0</v>
+      </c>
+      <c r="B299" s="1" t="n">
+        <v>0.8153416402546296</v>
+      </c>
+      <c r="C299" t="n">
+        <v>84</v>
+      </c>
+      <c r="D299" t="n">
+        <v>0.064</v>
+      </c>
+      <c r="E299" t="n">
+        <v>7.62</v>
+      </c>
+      <c r="F299" t="n">
+        <v>0.48768</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>3</v>
+      </c>
+      <c r="B300" s="1" t="n">
+        <v>0.8174209976851852</v>
+      </c>
+      <c r="C300" t="n">
+        <v>84</v>
+      </c>
+      <c r="D300" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E300" t="n">
+        <v>7.665</v>
+      </c>
+      <c r="F300" t="n">
+        <v>0.4599</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>6</v>
+      </c>
+      <c r="B301" s="1" t="n">
+        <v>0.8195034820023147</v>
+      </c>
+      <c r="C301" t="n">
+        <v>84</v>
+      </c>
+      <c r="D301" t="n">
+        <v>0.056</v>
+      </c>
+      <c r="E301" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="F301" t="n">
+        <v>0.4368</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>7</v>
+      </c>
+      <c r="B302" s="1" t="n">
+        <v>0.8201999172800927</v>
+      </c>
+      <c r="C302" t="n">
+        <v>84</v>
+      </c>
+      <c r="D302" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E302" t="n">
+        <v>7.92</v>
+      </c>
+      <c r="F302" t="n">
+        <v>0.4752</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>8</v>
+      </c>
+      <c r="B303" s="1" t="n">
+        <v>0.8208912117476851</v>
+      </c>
+      <c r="C303" t="n">
+        <v>84</v>
+      </c>
+      <c r="D303" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E303" t="n">
+        <v>8.055</v>
+      </c>
+      <c r="F303" t="n">
+        <v>0.4833</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>9</v>
+      </c>
+      <c r="B304" s="1" t="n">
+        <v>0.8215839490393519</v>
+      </c>
+      <c r="C304" t="n">
+        <v>84</v>
+      </c>
+      <c r="D304" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E304" t="n">
+        <v>8.174999999999999</v>
+      </c>
+      <c r="F304" t="n">
+        <v>0.4904999999999999</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>11</v>
+      </c>
+      <c r="B305" s="1" t="n">
+        <v>0.8229732221296296</v>
+      </c>
+      <c r="C305" t="n">
+        <v>84</v>
+      </c>
+      <c r="D305" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E305" t="n">
+        <v>8.01</v>
+      </c>
+      <c r="F305" t="n">
+        <v>0.4806</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>12</v>
+      </c>
+      <c r="B306" s="1" t="n">
+        <v>0.8236674721064815</v>
+      </c>
+      <c r="C306" t="n">
+        <v>84</v>
+      </c>
+      <c r="D306" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E306" t="n">
+        <v>7.935</v>
+      </c>
+      <c r="F306" t="n">
+        <v>0.4761</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>13</v>
+      </c>
+      <c r="B307" s="1" t="n">
+        <v>0.8243634315162036</v>
+      </c>
+      <c r="C307" t="n">
+        <v>84</v>
+      </c>
+      <c r="D307" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E307" t="n">
+        <v>7.904999999999999</v>
+      </c>
+      <c r="F307" t="n">
+        <v>0.4742999999999999</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>15</v>
+      </c>
+      <c r="B308" s="1" t="n">
+        <v>0.8257510431365741</v>
+      </c>
+      <c r="C308" t="n">
+        <v>84</v>
+      </c>
+      <c r="D308" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E308" t="n">
+        <v>8.084999999999999</v>
+      </c>
+      <c r="F308" t="n">
+        <v>0.4850999999999999</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>16</v>
+      </c>
+      <c r="B309" s="1" t="n">
+        <v>0.8264447633796297</v>
+      </c>
+      <c r="C309" t="n">
+        <v>84</v>
+      </c>
+      <c r="D309" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E309" t="n">
+        <v>8.295</v>
+      </c>
+      <c r="F309" t="n">
+        <v>0.4977</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>17</v>
+      </c>
+      <c r="B310" s="1" t="n">
+        <v>0.827136801875</v>
+      </c>
+      <c r="C310" t="n">
+        <v>84</v>
+      </c>
+      <c r="D310" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E310" t="n">
+        <v>8.01</v>
+      </c>
+      <c r="F310" t="n">
+        <v>0.4806</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>18</v>
+      </c>
+      <c r="B311" s="1" t="n">
+        <v>0.8278316803240741</v>
+      </c>
+      <c r="C311" t="n">
+        <v>84</v>
+      </c>
+      <c r="D311" t="n">
+        <v>0.056</v>
+      </c>
+      <c r="E311" t="n">
+        <v>7.425</v>
+      </c>
+      <c r="F311" t="n">
+        <v>0.4158</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>20</v>
+      </c>
+      <c r="B312" s="1" t="n">
+        <v>0.8292217640277778</v>
+      </c>
+      <c r="C312" t="n">
+        <v>84</v>
+      </c>
+      <c r="D312" t="n">
+        <v>0.052</v>
+      </c>
+      <c r="E312" t="n">
+        <v>6.84</v>
+      </c>
+      <c r="F312" t="n">
+        <v>0.35568</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>24</v>
+      </c>
+      <c r="B313" s="1" t="n">
+        <v>0.8319955449652778</v>
+      </c>
+      <c r="C313" t="n">
+        <v>84</v>
+      </c>
+      <c r="D313" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E313" t="n">
+        <v>6.12</v>
+      </c>
+      <c r="F313" t="n">
+        <v>0.26928</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>26</v>
+      </c>
+      <c r="B314" s="1" t="n">
+        <v>0.8333863175347223</v>
+      </c>
+      <c r="C314" t="n">
+        <v>84</v>
+      </c>
+      <c r="D314" t="n">
+        <v>0.056</v>
+      </c>
+      <c r="E314" t="n">
+        <v>7.755</v>
+      </c>
+      <c r="F314" t="n">
+        <v>0.43428</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>30</v>
+      </c>
+      <c r="B315" s="1" t="n">
+        <v>0.8361630832291667</v>
+      </c>
+      <c r="C315" t="n">
+        <v>84</v>
+      </c>
+      <c r="D315" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E315" t="n">
+        <v>6.18</v>
+      </c>
+      <c r="F315" t="n">
+        <v>0.27192</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>32</v>
+      </c>
+      <c r="B316" s="1" t="n">
+        <v>0.8375480725925927</v>
+      </c>
+      <c r="C316" t="n">
+        <v>84</v>
+      </c>
+      <c r="D316" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E316" t="n">
+        <v>6.12</v>
+      </c>
+      <c r="F316" t="n">
+        <v>0.26928</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
+        <v>33</v>
+      </c>
+      <c r="B317" s="1" t="n">
+        <v>0.8382421839351851</v>
+      </c>
+      <c r="C317" t="n">
+        <v>84</v>
+      </c>
+      <c r="D317" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E317" t="n">
+        <v>6.09</v>
+      </c>
+      <c r="F317" t="n">
+        <v>0.26796</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
+        <v>37</v>
+      </c>
+      <c r="B318" s="1" t="n">
+        <v>0.8410189341087962</v>
+      </c>
+      <c r="C318" t="n">
+        <v>84</v>
+      </c>
+      <c r="D318" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E318" t="n">
+        <v>6.315</v>
+      </c>
+      <c r="F318" t="n">
+        <v>0.2778599999999999</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="n">
+        <v>41</v>
+      </c>
+      <c r="B319" s="1" t="n">
+        <v>0.8437958049768519</v>
+      </c>
+      <c r="C319" t="n">
+        <v>84</v>
+      </c>
+      <c r="D319" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E319" t="n">
+        <v>5.535</v>
+      </c>
+      <c r="F319" t="n">
+        <v>0.2214</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
+        <v>45</v>
+      </c>
+      <c r="B320" s="1" t="n">
+        <v>0.8465734767592593</v>
+      </c>
+      <c r="C320" t="n">
+        <v>84</v>
+      </c>
+      <c r="D320" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="E320" t="n">
+        <v>6.524999999999999</v>
+      </c>
+      <c r="F320" t="n">
+        <v>0.3132</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="n">
+        <v>50</v>
+      </c>
+      <c r="B321" s="1" t="n">
+        <v>0.850045056863426</v>
+      </c>
+      <c r="C321" t="n">
+        <v>84</v>
+      </c>
+      <c r="D321" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E321" t="n">
+        <v>7.859999999999999</v>
+      </c>
+      <c r="F321" t="n">
+        <v>0.4716</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="n">
+        <v>51</v>
+      </c>
+      <c r="B322" s="1" t="n">
+        <v>0.8507408765509259</v>
+      </c>
+      <c r="C322" t="n">
+        <v>84</v>
+      </c>
+      <c r="D322" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="E322" t="n">
+        <v>8.594999999999999</v>
+      </c>
+      <c r="F322" t="n">
+        <v>0.58446</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
+        <v>54</v>
+      </c>
+      <c r="B323" s="1" t="n">
+        <v>0.8528180023379629</v>
+      </c>
+      <c r="C323" t="n">
+        <v>84</v>
+      </c>
+      <c r="D323" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="E323" t="n">
+        <v>8.265000000000001</v>
+      </c>
+      <c r="F323" t="n">
+        <v>0.5620200000000001</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="n">
+        <v>56</v>
+      </c>
+      <c r="B324" s="1" t="n">
+        <v>0.8542065822916667</v>
+      </c>
+      <c r="C324" t="n">
+        <v>84</v>
+      </c>
+      <c r="D324" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="E324" t="n">
+        <v>7.965</v>
+      </c>
+      <c r="F324" t="n">
+        <v>0.54162</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>57</v>
+      </c>
+      <c r="B325" s="1" t="n">
+        <v>0.8549042244791666</v>
+      </c>
+      <c r="C325" t="n">
+        <v>84</v>
+      </c>
+      <c r="D325" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="E325" t="n">
+        <v>7.904999999999999</v>
+      </c>
+      <c r="F325" t="n">
+        <v>0.53754</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>64</v>
+      </c>
+      <c r="B326" s="1" t="n">
+        <v>0.8597626139930556</v>
+      </c>
+      <c r="C326" t="n">
+        <v>84</v>
+      </c>
+      <c r="D326" t="n">
+        <v>0.07200000000000001</v>
+      </c>
+      <c r="E326" t="n">
+        <v>8.25</v>
+      </c>
+      <c r="F326" t="n">
+        <v>0.5940000000000001</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>65</v>
+      </c>
+      <c r="B327" s="1" t="n">
+        <v>0.8604528700925926</v>
+      </c>
+      <c r="C327" t="n">
+        <v>84</v>
+      </c>
+      <c r="D327" t="n">
+        <v>0.07200000000000001</v>
+      </c>
+      <c r="E327" t="n">
+        <v>8.279999999999999</v>
+      </c>
+      <c r="F327" t="n">
+        <v>0.59616</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>69</v>
+      </c>
+      <c r="B328" s="1" t="n">
+        <v>0.8632298105439814</v>
+      </c>
+      <c r="C328" t="n">
+        <v>84</v>
+      </c>
+      <c r="D328" t="n">
+        <v>0.07200000000000001</v>
+      </c>
+      <c r="E328" t="n">
+        <v>8.504999999999999</v>
+      </c>
+      <c r="F328" t="n">
+        <v>0.61236</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="n">
+        <v>70</v>
+      </c>
+      <c r="B329" s="1" t="n">
+        <v>0.8639226295601852</v>
+      </c>
+      <c r="C329" t="n">
+        <v>84</v>
+      </c>
+      <c r="D329" t="n">
+        <v>0.07200000000000001</v>
+      </c>
+      <c r="E329" t="n">
+        <v>8.504999999999999</v>
+      </c>
+      <c r="F329" t="n">
+        <v>0.61236</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="n">
+        <v>71</v>
+      </c>
+      <c r="B330" s="1" t="n">
+        <v>0.8646267941203704</v>
+      </c>
+      <c r="C330" t="n">
+        <v>84</v>
+      </c>
+      <c r="D330" t="n">
+        <v>0.07200000000000001</v>
+      </c>
+      <c r="E330" t="n">
+        <v>8.52</v>
+      </c>
+      <c r="F330" t="n">
+        <v>0.6134400000000001</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="n">
+        <v>76</v>
+      </c>
+      <c r="B331" s="1" t="n">
+        <v>0.8680876039583333</v>
+      </c>
+      <c r="C331" t="n">
+        <v>84</v>
+      </c>
+      <c r="D331" t="n">
+        <v>0.052</v>
+      </c>
+      <c r="E331" t="n">
+        <v>5.819999999999999</v>
+      </c>
+      <c r="F331" t="n">
+        <v>0.30264</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="n">
+        <v>77</v>
+      </c>
+      <c r="B332" s="1" t="n">
+        <v>0.8687819911111112</v>
+      </c>
+      <c r="C332" t="n">
+        <v>84</v>
+      </c>
+      <c r="D332" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="E332" t="n">
+        <v>5.565</v>
+      </c>
+      <c r="F332" t="n">
+        <v>0.26712</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="n">
+        <v>78</v>
+      </c>
+      <c r="B333" s="1" t="n">
+        <v>0.8694753972106481</v>
+      </c>
+      <c r="C333" t="n">
+        <v>84</v>
+      </c>
+      <c r="D333" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="E333" t="n">
+        <v>5.475</v>
+      </c>
+      <c r="F333" t="n">
+        <v>0.2628</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="n">
+        <v>80</v>
+      </c>
+      <c r="B334" s="1" t="n">
+        <v>0.8708684543749999</v>
+      </c>
+      <c r="C334" t="n">
+        <v>84</v>
+      </c>
+      <c r="D334" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E334" t="n">
+        <v>6.975</v>
+      </c>
+      <c r="F334" t="n">
+        <v>0.4185</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="n">
+        <v>82</v>
+      </c>
+      <c r="B335" s="1" t="n">
+        <v>0.8722546081597221</v>
+      </c>
+      <c r="C335" t="n">
+        <v>84</v>
+      </c>
+      <c r="D335" t="n">
+        <v>0.052</v>
+      </c>
+      <c r="E335" t="n">
+        <v>6.165</v>
+      </c>
+      <c r="F335" t="n">
+        <v>0.32058</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="n">
+        <v>83</v>
+      </c>
+      <c r="B336" s="1" t="n">
+        <v>0.8729464328472223</v>
+      </c>
+      <c r="C336" t="n">
+        <v>84</v>
+      </c>
+      <c r="D336" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="E336" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="F336" t="n">
+        <v>0.26352</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="n">
+        <v>84</v>
+      </c>
+      <c r="B337" s="1" t="n">
+        <v>0.8736403583796297</v>
+      </c>
+      <c r="C337" t="n">
+        <v>84</v>
+      </c>
+      <c r="D337" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="E337" t="n">
+        <v>5.654999999999999</v>
+      </c>
+      <c r="F337" t="n">
+        <v>0.27144</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="n">
+        <v>86</v>
+      </c>
+      <c r="B338" s="1" t="n">
+        <v>0.8750293881250001</v>
+      </c>
+      <c r="C338" t="n">
+        <v>84</v>
+      </c>
+      <c r="D338" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="E338" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="F338" t="n">
+        <v>0.26352</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="n">
+        <v>87</v>
+      </c>
+      <c r="B339" s="1" t="n">
+        <v>0.8757234395023148</v>
+      </c>
+      <c r="C339" t="n">
+        <v>84</v>
+      </c>
+      <c r="D339" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="E339" t="n">
+        <v>5.34</v>
+      </c>
+      <c r="F339" t="n">
+        <v>0.25632</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="n">
+        <v>90</v>
+      </c>
+      <c r="B340" s="1" t="n">
+        <v>0.877804328587963</v>
+      </c>
+      <c r="C340" t="n">
+        <v>84</v>
+      </c>
+      <c r="D340" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E340" t="n">
+        <v>4.965</v>
+      </c>
+      <c r="F340" t="n">
+        <v>0.21846</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="n">
+        <v>91</v>
+      </c>
+      <c r="B341" s="1" t="n">
+        <v>0.8784981737847223</v>
+      </c>
+      <c r="C341" t="n">
+        <v>84</v>
+      </c>
+      <c r="D341" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E341" t="n">
+        <v>4.875</v>
+      </c>
+      <c r="F341" t="n">
+        <v>0.2145</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="n">
+        <v>93</v>
+      </c>
+      <c r="B342" s="1" t="n">
+        <v>0.8798870867824075</v>
+      </c>
+      <c r="C342" t="n">
+        <v>84</v>
+      </c>
+      <c r="D342" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E342" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="F342" t="n">
+        <v>0.2112</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="n">
+        <v>95</v>
+      </c>
+      <c r="B343" s="1" t="n">
+        <v>0.8812779949074074</v>
+      </c>
+      <c r="C343" t="n">
+        <v>84</v>
+      </c>
+      <c r="D343" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E343" t="n">
+        <v>4.68</v>
+      </c>
+      <c r="F343" t="n">
+        <v>0.20592</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="n">
+        <v>97</v>
+      </c>
+      <c r="B344" s="1" t="n">
+        <v>0.882662464837963</v>
+      </c>
+      <c r="C344" t="n">
+        <v>84</v>
+      </c>
+      <c r="D344" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E344" t="n">
+        <v>4.605</v>
+      </c>
+      <c r="F344" t="n">
+        <v>0.20262</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="n">
+        <v>99</v>
+      </c>
+      <c r="B345" s="1" t="n">
+        <v>0.8840516996875</v>
+      </c>
+      <c r="C345" t="n">
+        <v>84</v>
+      </c>
+      <c r="D345" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E345" t="n">
+        <v>4.545</v>
+      </c>
+      <c r="F345" t="n">
+        <v>0.19998</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="n">
+        <v>100</v>
+      </c>
+      <c r="B346" s="1" t="n">
+        <v>0.8847449788657408</v>
+      </c>
+      <c r="C346" t="n">
+        <v>84</v>
+      </c>
+      <c r="D346" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E346" t="n">
+        <v>4.29</v>
+      </c>
+      <c r="F346" t="n">
+        <v>0.18876</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="n">
+        <v>102</v>
+      </c>
+      <c r="B347" s="1" t="n">
+        <v>0.8861353698726852</v>
+      </c>
+      <c r="C347" t="n">
+        <v>84</v>
+      </c>
+      <c r="D347" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E347" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="F347" t="n">
+        <v>0.18744</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="n">
+        <v>103</v>
+      </c>
+      <c r="B348" s="1" t="n">
+        <v>0.8868305428587964</v>
+      </c>
+      <c r="C348" t="n">
+        <v>84</v>
+      </c>
+      <c r="D348" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E348" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="F348" t="n">
+        <v>0.18744</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="n">
+        <v>105</v>
+      </c>
+      <c r="B349" s="1" t="n">
+        <v>0.8882160268055556</v>
+      </c>
+      <c r="C349" t="n">
+        <v>84</v>
+      </c>
+      <c r="D349" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E349" t="n">
+        <v>4.23</v>
+      </c>
+      <c r="F349" t="n">
+        <v>0.18612</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="n">
+        <v>106</v>
+      </c>
+      <c r="B350" s="1" t="n">
+        <v>0.8889095145601852</v>
+      </c>
+      <c r="C350" t="n">
+        <v>84</v>
+      </c>
+      <c r="D350" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E350" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="F350" t="n">
+        <v>0.1848</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="n">
+        <v>111</v>
+      </c>
+      <c r="B351" s="1" t="n">
+        <v>0.8923799532638889</v>
+      </c>
+      <c r="C351" t="n">
+        <v>84</v>
+      </c>
+      <c r="D351" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E351" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="F351" t="n">
+        <v>0.17556</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="n">
+        <v>112</v>
+      </c>
+      <c r="B352" s="1" t="n">
+        <v>0.8930741099537036</v>
+      </c>
+      <c r="C352" t="n">
+        <v>84</v>
+      </c>
+      <c r="D352" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E352" t="n">
+        <v>3.885</v>
+      </c>
+      <c r="F352" t="n">
+        <v>0.17094</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="n">
+        <v>113</v>
+      </c>
+      <c r="B353" s="1" t="n">
+        <v>0.8937677587847221</v>
+      </c>
+      <c r="C353" t="n">
+        <v>84</v>
+      </c>
+      <c r="D353" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E353" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="F353" t="n">
+        <v>0.1536</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="n">
+        <v>117</v>
+      </c>
+      <c r="B354" s="1" t="n">
+        <v>0.8965446894212962</v>
+      </c>
+      <c r="C354" t="n">
+        <v>84</v>
+      </c>
+      <c r="D354" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E354" t="n">
+        <v>3.63</v>
+      </c>
+      <c r="F354" t="n">
+        <v>0.1452</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="n">
+        <v>118</v>
+      </c>
+      <c r="B355" s="1" t="n">
+        <v>0.8972402992708333</v>
+      </c>
+      <c r="C355" t="n">
+        <v>84</v>
+      </c>
+      <c r="D355" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E355" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="F355" t="n">
+        <v>0.1428</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="n">
+        <v>121</v>
+      </c>
+      <c r="B356" s="1" t="n">
+        <v>0.8993207937731481</v>
+      </c>
+      <c r="C356" t="n">
+        <v>84</v>
+      </c>
+      <c r="D356" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E356" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="F356" t="n">
+        <v>0.138</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="n">
+        <v>125</v>
+      </c>
+      <c r="B357" s="1" t="n">
+        <v>0.9020972359837963</v>
+      </c>
+      <c r="C357" t="n">
+        <v>84</v>
+      </c>
+      <c r="D357" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E357" t="n">
+        <v>3.345</v>
+      </c>
+      <c r="F357" t="n">
+        <v>0.14718</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="n">
+        <v>126</v>
+      </c>
+      <c r="B358" s="1" t="n">
+        <v>0.9027914582060186</v>
+      </c>
+      <c r="C358" t="n">
+        <v>84</v>
+      </c>
+      <c r="D358" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E358" t="n">
+        <v>3.315</v>
+      </c>
+      <c r="F358" t="n">
+        <v>0.14586</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="n">
+        <v>128</v>
+      </c>
+      <c r="B359" s="1" t="n">
+        <v>0.9041786980324075</v>
+      </c>
+      <c r="C359" t="n">
+        <v>84</v>
+      </c>
+      <c r="D359" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E359" t="n">
+        <v>3.255</v>
+      </c>
+      <c r="F359" t="n">
+        <v>0.14322</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="n">
+        <v>131</v>
+      </c>
+      <c r="B360" s="1" t="n">
+        <v>0.9062622866087963</v>
+      </c>
+      <c r="C360" t="n">
+        <v>84</v>
+      </c>
+      <c r="D360" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E360" t="n">
+        <v>3.195</v>
+      </c>
+      <c r="F360" t="n">
+        <v>0.1278</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="n">
+        <v>132</v>
+      </c>
+      <c r="B361" s="1" t="n">
+        <v>0.9069594801041667</v>
+      </c>
+      <c r="C361" t="n">
+        <v>84</v>
+      </c>
+      <c r="D361" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E361" t="n">
+        <v>3.18</v>
+      </c>
+      <c r="F361" t="n">
+        <v>0.1272</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="n">
+        <v>134</v>
+      </c>
+      <c r="B362" s="1" t="n">
+        <v>0.9083453346990741</v>
+      </c>
+      <c r="C362" t="n">
+        <v>84</v>
+      </c>
+      <c r="D362" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E362" t="n">
+        <v>3.225</v>
+      </c>
+      <c r="F362" t="n">
+        <v>0.1419</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="n">
+        <v>136</v>
+      </c>
+      <c r="B363" s="1" t="n">
+        <v>0.9097330809374999</v>
+      </c>
+      <c r="C363" t="n">
+        <v>84</v>
+      </c>
+      <c r="D363" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E363" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="F363" t="n">
+        <v>0.14256</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="n">
+        <v>137</v>
+      </c>
+      <c r="B364" s="1" t="n">
+        <v>0.9104252291203703</v>
+      </c>
+      <c r="C364" t="n">
+        <v>84</v>
+      </c>
+      <c r="D364" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E364" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="F364" t="n">
+        <v>0.14256</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="n">
+        <v>138</v>
+      </c>
+      <c r="B365" s="1" t="n">
+        <v>0.9111226987037038</v>
+      </c>
+      <c r="C365" t="n">
+        <v>84</v>
+      </c>
+      <c r="D365" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E365" t="n">
+        <v>3.255</v>
+      </c>
+      <c r="F365" t="n">
+        <v>0.14322</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="n">
+        <v>139</v>
+      </c>
+      <c r="B366" s="1" t="n">
+        <v>0.9118144540162038</v>
+      </c>
+      <c r="C366" t="n">
+        <v>84</v>
+      </c>
+      <c r="D366" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E366" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="F366" t="n">
+        <v>0.14256</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="n">
+        <v>150</v>
+      </c>
+      <c r="B367" s="1" t="n">
+        <v>0.9194475210648149</v>
+      </c>
+      <c r="C367" t="n">
+        <v>84</v>
+      </c>
+      <c r="D367" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="E367" t="n">
+        <v>4.245</v>
+      </c>
+      <c r="F367" t="n">
+        <v>0.20376</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="n">
+        <v>152</v>
+      </c>
+      <c r="B368" s="1" t="n">
+        <v>0.9208370923842593</v>
+      </c>
+      <c r="C368" t="n">
+        <v>84</v>
+      </c>
+      <c r="D368" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="E368" t="n">
+        <v>4.215</v>
+      </c>
+      <c r="F368" t="n">
+        <v>0.20232</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="n">
+        <v>154</v>
+      </c>
+      <c r="B369" s="1" t="n">
+        <v>0.9222250234953703</v>
+      </c>
+      <c r="C369" t="n">
+        <v>84</v>
+      </c>
+      <c r="D369" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="E369" t="n">
+        <v>4.109999999999999</v>
+      </c>
+      <c r="F369" t="n">
+        <v>0.19728</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="n">
+        <v>157</v>
+      </c>
+      <c r="B370" s="1" t="n">
+        <v>0.9243063936226852</v>
+      </c>
+      <c r="C370" t="n">
+        <v>84</v>
+      </c>
+      <c r="D370" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E370" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="F370" t="n">
+        <v>0.16896</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="n">
+        <v>158</v>
+      </c>
+      <c r="B371" s="1" t="n">
+        <v>0.9250034248958333</v>
+      </c>
+      <c r="C371" t="n">
+        <v>84</v>
+      </c>
+      <c r="D371" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E371" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="F371" t="n">
+        <v>0.1512</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="n">
+        <v>163</v>
+      </c>
+      <c r="B372" s="1" t="n">
+        <v>0.9284730395486112</v>
+      </c>
+      <c r="C372" t="n">
+        <v>84</v>
+      </c>
+      <c r="D372" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E372" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="F372" t="n">
+        <v>0.1332</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="n">
+        <v>167</v>
+      </c>
+      <c r="B373" s="1" t="n">
+        <v>0.931249435625</v>
+      </c>
+      <c r="C373" t="n">
+        <v>84</v>
+      </c>
+      <c r="D373" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E373" t="n">
+        <v>3.03</v>
+      </c>
+      <c r="F373" t="n">
+        <v>0.13332</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="n">
+        <v>168</v>
+      </c>
+      <c r="B374" s="1" t="n">
+        <v>0.9319421370254629</v>
+      </c>
+      <c r="C374" t="n">
+        <v>84</v>
+      </c>
+      <c r="D374" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="E374" t="n">
+        <v>2.955</v>
+      </c>
+      <c r="F374" t="n">
+        <v>0.13002</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="n">
+        <v>171</v>
+      </c>
+      <c r="B375" s="1" t="n">
+        <v>0.934024604849537</v>
+      </c>
+      <c r="C375" t="n">
+        <v>84</v>
+      </c>
+      <c r="D375" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E375" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="F375" t="n">
+        <v>0.1116</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="n">
+        <v>172</v>
+      </c>
+      <c r="B376" s="1" t="n">
+        <v>0.9347183012615742</v>
+      </c>
+      <c r="C376" t="n">
+        <v>84</v>
+      </c>
+      <c r="D376" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E376" t="n">
+        <v>2.715</v>
+      </c>
+      <c r="F376" t="n">
+        <v>0.1086</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="n">
+        <v>173</v>
+      </c>
+      <c r="B377" s="1" t="n">
+        <v>0.9354126885300926</v>
+      </c>
+      <c r="C377" t="n">
+        <v>84</v>
+      </c>
+      <c r="D377" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E377" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="F377" t="n">
+        <v>0.1056</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="n">
+        <v>175</v>
+      </c>
+      <c r="B378" s="1" t="n">
+        <v>0.93680322875</v>
+      </c>
+      <c r="C378" t="n">
+        <v>84</v>
+      </c>
+      <c r="D378" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E378" t="n">
+        <v>2.475</v>
+      </c>
+      <c r="F378" t="n">
+        <v>0.099</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="n">
+        <v>180</v>
+      </c>
+      <c r="B379" s="1" t="n">
+        <v>0.9402724514467592</v>
+      </c>
+      <c r="C379" t="n">
+        <v>84</v>
+      </c>
+      <c r="D379" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="E379" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="F379" t="n">
+        <v>0.0624</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="n">
+        <v>182</v>
+      </c>
+      <c r="B380" s="1" t="n">
+        <v>0.9416605903472222</v>
+      </c>
+      <c r="C380" t="n">
+        <v>84</v>
+      </c>
+      <c r="D380" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="E380" t="n">
+        <v>1.515</v>
+      </c>
+      <c r="F380" t="n">
+        <v>0.04242</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="n">
+        <v>184</v>
+      </c>
+      <c r="B381" s="1" t="n">
+        <v>0.9430520194560185</v>
+      </c>
+      <c r="C381" t="n">
+        <v>84</v>
+      </c>
+      <c r="D381" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="E381" t="n">
+        <v>1.245</v>
+      </c>
+      <c r="F381" t="n">
+        <v>0.02988</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="n">
+        <v>188</v>
+      </c>
+      <c r="B382" s="1" t="n">
+        <v>0.9458232790277777</v>
+      </c>
+      <c r="C382" t="n">
+        <v>84</v>
+      </c>
+      <c r="D382" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E382" t="n">
+        <v>0.975</v>
+      </c>
+      <c r="F382" t="n">
+        <v>0.0195</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="n">
+        <v>190</v>
+      </c>
+      <c r="B383" s="1" t="n">
+        <v>0.9472129894560184</v>
+      </c>
+      <c r="C383" t="n">
+        <v>84</v>
+      </c>
+      <c r="D383" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E383" t="n">
+        <v>0.9299999999999999</v>
+      </c>
+      <c r="F383" t="n">
+        <v>0.0186</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="n">
+        <v>192</v>
+      </c>
+      <c r="B384" s="1" t="n">
+        <v>0.9485989600810185</v>
+      </c>
+      <c r="C384" t="n">
+        <v>84</v>
+      </c>
+      <c r="D384" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E384" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="F384" t="n">
+        <v>0.0171</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="n">
+        <v>193</v>
+      </c>
+      <c r="B385" s="1" t="n">
+        <v>0.9492934962268518</v>
+      </c>
+      <c r="C385" t="n">
+        <v>84</v>
+      </c>
+      <c r="D385" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="E385" t="n">
+        <v>0.8099999999999999</v>
+      </c>
+      <c r="F385" t="n">
+        <v>0.01296</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="n">
+        <v>194</v>
+      </c>
+      <c r="B386" s="1" t="n">
+        <v>0.9499881041898148</v>
+      </c>
+      <c r="C386" t="n">
+        <v>84</v>
+      </c>
+      <c r="D386" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="E386" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="F386" t="n">
+        <v>0.01248</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="n">
+        <v>196</v>
+      </c>
+      <c r="B387" s="1" t="n">
+        <v>0.9513759904861111</v>
+      </c>
+      <c r="C387" t="n">
+        <v>84</v>
+      </c>
+      <c r="D387" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="E387" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="F387" t="n">
+        <v>0.01152</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="n">
+        <v>198</v>
+      </c>
+      <c r="B388" s="1" t="n">
+        <v>0.952765213900463</v>
+      </c>
+      <c r="C388" t="n">
+        <v>84</v>
+      </c>
+      <c r="D388" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="E388" t="n">
+        <v>0.6749999999999999</v>
+      </c>
+      <c r="F388" t="n">
+        <v>0.0108</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="n">
+        <v>202</v>
+      </c>
+      <c r="B389" s="1" t="n">
+        <v>0.9555400949421295</v>
+      </c>
+      <c r="C389" t="n">
+        <v>84</v>
+      </c>
+      <c r="D389" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="E389" t="n">
+        <v>0.585</v>
+      </c>
+      <c r="F389" t="n">
+        <v>0.00936</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="n">
+        <v>204</v>
+      </c>
+      <c r="B390" s="1" t="n">
+        <v>0.9569281633796296</v>
+      </c>
+      <c r="C390" t="n">
+        <v>84</v>
+      </c>
+      <c r="D390" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="E390" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="F390" t="n">
+        <v>0.01008</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="n">
+        <v>207</v>
+      </c>
+      <c r="B391" s="1" t="n">
+        <v>0.9590100010763889</v>
+      </c>
+      <c r="C391" t="n">
+        <v>84</v>
+      </c>
+      <c r="D391" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="E391" t="n">
+        <v>0.585</v>
+      </c>
+      <c r="F391" t="n">
+        <v>0.00936</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="n">
+        <v>208</v>
+      </c>
+      <c r="B392" s="1" t="n">
+        <v>0.9597061547800926</v>
+      </c>
+      <c r="C392" t="n">
+        <v>84</v>
+      </c>
+      <c r="D392" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="E392" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="F392" t="n">
+        <v>0.00864</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="n">
+        <v>209</v>
+      </c>
+      <c r="B393" s="1" t="n">
+        <v>0.9603981787847222</v>
+      </c>
+      <c r="C393" t="n">
+        <v>84</v>
+      </c>
+      <c r="D393" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="E393" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="F393" t="n">
+        <v>0.008160000000000001</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="n">
+        <v>210</v>
+      </c>
+      <c r="B394" s="1" t="n">
+        <v>0.961096224224537</v>
+      </c>
+      <c r="C394" t="n">
+        <v>84</v>
+      </c>
+      <c r="D394" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="E394" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="F394" t="n">
+        <v>0.005759999999999999</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="n">
+        <v>211</v>
+      </c>
+      <c r="B395" s="1" t="n">
+        <v>0.9617866515393519</v>
+      </c>
+      <c r="C395" t="n">
+        <v>84</v>
+      </c>
+      <c r="D395" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="E395" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="F395" t="n">
+        <v>0.005759999999999999</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="n">
+        <v>220</v>
+      </c>
+      <c r="B396" s="1" t="n">
+        <v>0.9680362659722221</v>
+      </c>
+      <c r="C396" t="n">
+        <v>84</v>
+      </c>
+      <c r="D396" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="E396" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="F396" t="n">
+        <v>0.00468</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="n">
+        <v>221</v>
+      </c>
+      <c r="B397" s="1" t="n">
+        <v>0.9687273288541667</v>
+      </c>
+      <c r="C397" t="n">
+        <v>84</v>
+      </c>
+      <c r="D397" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="E397" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F397" t="n">
+        <v>0.004500000000000001</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="n">
+        <v>230</v>
+      </c>
+      <c r="B398" s="1" t="n">
+        <v>0.9749739801967593</v>
+      </c>
+      <c r="C398" t="n">
+        <v>84</v>
+      </c>
+      <c r="D398" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="E398" t="n">
+        <v>0.285</v>
+      </c>
+      <c r="F398" t="n">
+        <v>0.00342</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="n">
+        <v>235</v>
+      </c>
+      <c r="B399" s="1" t="n">
+        <v>0.9784455207638889</v>
+      </c>
+      <c r="C399" t="n">
+        <v>84</v>
+      </c>
+      <c r="D399" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="E399" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="F399" t="n">
+        <v>0.00252</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="n">
+        <v>236</v>
+      </c>
+      <c r="B400" s="1" t="n">
+        <v>0.9791381067708333</v>
+      </c>
+      <c r="C400" t="n">
+        <v>84</v>
+      </c>
+      <c r="D400" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="E400" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="F400" t="n">
+        <v>0.00216</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="n">
+        <v>242</v>
+      </c>
+      <c r="B401" s="1" t="n">
+        <v>0.9833025013773148</v>
+      </c>
+      <c r="C401" t="n">
+        <v>84</v>
+      </c>
+      <c r="D401" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="E401" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="F401" t="n">
+        <v>0.0012</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="n">
+        <v>246</v>
+      </c>
+      <c r="B402" s="1" t="n">
+        <v>0.9860785783796296</v>
+      </c>
+      <c r="C402" t="n">
+        <v>84</v>
+      </c>
+      <c r="D402" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="E402" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="F402" t="n">
+        <v>0.00096</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="n">
+        <v>249</v>
+      </c>
+      <c r="B403" s="1" t="n">
+        <v>0.9881618087847222</v>
+      </c>
+      <c r="C403" t="n">
+        <v>84</v>
+      </c>
+      <c r="D403" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="E403" t="n">
+        <v>0.105</v>
+      </c>
+      <c r="F403" t="n">
+        <v>0.00084</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="n">
+        <v>251</v>
+      </c>
+      <c r="B404" s="1" t="n">
+        <v>0.9895511357523148</v>
+      </c>
+      <c r="C404" t="n">
+        <v>84</v>
+      </c>
+      <c r="D404" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="E404" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="F404" t="n">
+        <v>0.0007199999999999999</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="n">
+        <v>253</v>
+      </c>
+      <c r="B405" s="1" t="n">
+        <v>0.9909423334722223</v>
+      </c>
+      <c r="C405" t="n">
+        <v>84</v>
+      </c>
+      <c r="D405" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="E405" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="F405" t="n">
+        <v>0.0007199999999999999</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="n">
+        <v>4</v>
+      </c>
+      <c r="B406" s="1" t="n">
+        <v>0.9951020066666667</v>
+      </c>
+      <c r="C406" t="n">
+        <v>84</v>
+      </c>
+      <c r="D406" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="E406" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="F406" t="n">
+        <v>0.0005999999999999999</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="n">
+        <v>6</v>
+      </c>
+      <c r="B407" s="1" t="n">
+        <v>0.9964902973958333</v>
+      </c>
+      <c r="C407" t="n">
+        <v>84</v>
+      </c>
+      <c r="D407" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="E407" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="F407" t="n">
+        <v>0.0007199999999999999</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="n">
+        <v>8</v>
+      </c>
+      <c r="B408" s="1" t="n">
+        <v>0.9978802621875</v>
+      </c>
+      <c r="C408" t="n">
+        <v>84</v>
+      </c>
+      <c r="D408" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="E408" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="F408" t="n">
+        <v>0.0005999999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>